<commit_message>
Update to styling: trying to add images to answer pages but have been unable to get it to work
</commit_message>
<xml_diff>
--- a/AnswerKey.xlsx
+++ b/AnswerKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marshall's Laptop\Documents\U of R Coding Bootcamp\02_Homework\Module05\TriviaGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EA6352-1AFE-4DD9-A580-96C1AEA981EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6111CD1B-7A77-44A4-A54B-690E98CF836E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21924" windowHeight="9576" xr2:uid="{F509D299-CD78-4140-96BF-1B4FA20734F6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11412" xr2:uid="{F509D299-CD78-4140-96BF-1B4FA20734F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
   <si>
     <t>Unit 5 - Trivia Game Answer Key</t>
   </si>
@@ -152,18 +152,6 @@
     <t xml:space="preserve">    { q: "What is the smallest border between two countries (including exclaves)?"</t>
   </si>
   <si>
-    <t xml:space="preserve"> answers: [{a: "Georgia/Armenia"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {a: "Spain/Morocco"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {a: "Malaysia/Singapore"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {a: "England/France"</t>
-  </si>
-  <si>
     <t xml:space="preserve">    { q: "What is the lowest point on land in the world?"</t>
   </si>
   <si>
@@ -179,9 +167,6 @@
     <t xml:space="preserve"> {a: "Lagunda del Carbon"</t>
   </si>
   <si>
-    <t xml:space="preserve">    { q: "The top ten highest peaks in the world are in the same mountain range. Which mountain range are they located in?"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> answers: [{a: "Himalayas"</t>
   </si>
   <si>
@@ -218,10 +203,85 @@
     <t xml:space="preserve"> {a: "Italy"</t>
   </si>
   <si>
-    <t>Image File</t>
-  </si>
-  <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Rome,+Metropolitan+City+of+Rome,+Italy/@41.8315011,12.382721,5.73z/data=!4m5!3m4!1s0x132f6196f9928ebb:0xb90f770693656e38!8m2!3d41.9027835!4d12.4963655</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=when+did+rome+become+the+capital+of+italy&amp;oq=when+did+rome+become+the&amp;aqs=chrome.0.0j69i57j0l4.12531j0j7&amp;sourceid=chrome&amp;ie=UTF-8</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Dead+Sea/@31.4640471,36.1477255,7z/data=!4m5!3m4!1s0x15033c2eaf9fbba1:0xf38cff48a0c15882!8m2!3d31.5590287!4d35.4731895</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/deva/learn/nature/lowest-places-on-earth.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    { q: "Nine of the top ten highest peaks in the world are in the same mountain range. Which mountain range are they located in?"</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_highest_mountains_on_Earth</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Himalayas/@28.9094507,83.5987005,5.26z/data=!4m5!3m4!1s0x3995b9ebef1235bd:0x3ae1297b70640201!8m2!3d28.5983159!4d83.9310623</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/French+Guiana/@1.1024713,-53.2776219,5.75z/data=!4m5!3m4!1s0x8d12155785f7d753:0xde27f7e90f0af446!8m2!3d3.933889!4d-53.125782</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/French_Guiana</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/United+Arab+Emirates/@24.1975601,53.7723288,6z/data=!4m5!3m4!1s0x3e5e48dfb1ab12bd:0x33d32f56c0080aa7!8m2!3d23.424076!4d53.847818</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_countries_by_GDP_(nominal)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/United_Arab_Emirates#Economy</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/United+States/@41.3420278,-106.0689691,3.61z/data=!4m5!3m4!1s0x54eab584e432360b:0x1c3bb99243deb742!8m2!3d37.09024!4d-95.712891</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=when+did+italy+unify&amp;oq=when+did+italy+u&amp;aqs=chrome.1.69i57j0l5.4996j1j4&amp;sourceid=chrome&amp;ie=UTF-8</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?hl=en&amp;source=hp&amp;ei=VIEMXNGlBsWQ5gLJz4ugAg&amp;q=when+did+germany+unify&amp;btnK=Google+Search&amp;oq=when+did+ger&amp;gs_l=psy-ab.3.0.0i67j0l9.13542.14990..15908...1.0..0.100.1171.12j1....3..0....1..gws-wiz.....0..35i39j0i131.-pia0no251M</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Norway/@63.6059669,11.6990547,4.23z/data=!4m5!3m4!1s0x461268458f4de5bf:0xa1b03b9db864d02b!8m2!3d60.472024!4d8.468946</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_countries_by_length_of_coastline</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_countries_and_territories_by_land_borders</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/@57.8928913,83.1369811,3z</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Botswana/@-17.78735,25.2577052,12.75z/data=!4m5!3m4!1s0x1ea44321d1452211:0xf1647c2a8715af7b!8m2!3d-22.328474!4d24.684866</t>
+  </si>
+  <si>
+    <t>https://garfors.com/2013/07/the-worlds-11-shortest-land-borders-html/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {a: "Botswana-Zambia"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {a: "Croatia-Montenegro"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {a: "Armenia-Iran"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> answers: [{a: "Egypt-Palestine"</t>
   </si>
 </sst>
 </file>
@@ -265,10 +325,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,36 +644,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2831717D-9C8D-4ED0-94BB-D961EB02906B}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4656" ySplit="1152" topLeftCell="C4" activePane="topRight"/>
-      <selection pane="topRight" activeCell="L3" sqref="L3"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <pane xSplit="4656" ySplit="1152" topLeftCell="B4" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1:L1048576"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="1.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -641,13 +702,13 @@
         <v>9</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -675,95 +736,131 @@
       <c r="I4" t="s">
         <v>17</v>
       </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
       </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>65</v>
+      </c>
+      <c r="M6" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
       </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -791,66 +888,102 @@
       <c r="I8" t="s">
         <v>17</v>
       </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N8" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
       </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="K10">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -858,7 +991,7 @@
         <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>51</v>
@@ -870,7 +1003,7 @@
         <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>53</v>
@@ -878,66 +1011,90 @@
       <c r="I11" t="s">
         <v>17</v>
       </c>
+      <c r="K11">
+        <v>8</v>
+      </c>
+      <c r="L11" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
       </c>
+      <c r="K12">
+        <v>9</v>
+      </c>
+      <c r="L12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
         <v>14</v>
       </c>
-      <c r="F13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
       </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L13">
+    <sortCondition ref="K4:K13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>